<commit_message>
Added velella and pyrosome findings from calcofi
</commit_message>
<xml_diff>
--- a/data/CalCOFI Coding Form (Responses).xlsx
+++ b/data/CalCOFI Coding Form (Responses).xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1632" uniqueCount="458">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1689" uniqueCount="468">
   <si>
     <t>Timestamp</t>
   </si>
@@ -1419,6 +1419,36 @@
   </si>
   <si>
     <t>summer and fall 2014, and again in early 2015</t>
+  </si>
+  <si>
+    <t>Pyrosomes</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Oregon (Newport Hydrographic Line)</t>
+  </si>
+  <si>
+    <t>first observed in the fall of 2016</t>
+  </si>
+  <si>
+    <t>fall</t>
+  </si>
+  <si>
+    <t>tropical species</t>
+  </si>
+  <si>
+    <t>Phacellophora camchatica</t>
+  </si>
+  <si>
+    <t>Northern California Current, Oregon and Washington Coast</t>
+  </si>
+  <si>
+    <t>offshore and/or southern species</t>
+  </si>
+  <si>
+    <t>Velella velella</t>
+  </si>
+  <si>
+    <t>Thetys</t>
   </si>
 </sst>
 </file>
@@ -1798,7 +1828,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:IW74" displayName="Form_Responses1" name="Form_Responses1" id="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:IW76" displayName="Form_Responses1" name="Form_Responses1" id="1">
   <tableColumns count="257">
     <tableColumn name="Timestamp" id="1"/>
     <tableColumn name="Email Address" id="2"/>
@@ -10340,104 +10370,339 @@
       </c>
     </row>
     <row r="74">
-      <c r="A74" s="31">
+      <c r="A74" s="14">
         <v>45838.52682344908</v>
       </c>
-      <c r="B74" s="32" t="s">
+      <c r="B74" s="15" t="s">
         <v>403</v>
       </c>
-      <c r="C74" s="32" t="s">
+      <c r="C74" s="15" t="s">
         <v>404</v>
       </c>
-      <c r="D74" s="32">
+      <c r="D74" s="15">
         <v>73.0</v>
       </c>
-      <c r="E74" s="32" t="s">
+      <c r="E74" s="15" t="s">
         <v>261</v>
       </c>
-      <c r="H74" s="32" t="s">
+      <c r="H74" s="15" t="s">
         <v>431</v>
       </c>
-      <c r="I74" s="32" t="s">
+      <c r="I74" s="15" t="s">
         <v>263</v>
       </c>
-      <c r="J74" s="32" t="s">
-        <v>264</v>
-      </c>
-      <c r="K74" s="32" t="s">
+      <c r="J74" s="15" t="s">
+        <v>264</v>
+      </c>
+      <c r="K74" s="15" t="s">
         <v>265</v>
       </c>
-      <c r="O74" s="32" t="s">
+      <c r="O74" s="15" t="s">
         <v>456</v>
       </c>
-      <c r="P74" s="32">
+      <c r="P74" s="15">
         <v>41.0518</v>
       </c>
-      <c r="Q74" s="32" t="s">
-        <v>267</v>
-      </c>
-      <c r="R74" s="32" t="s">
+      <c r="Q74" s="15" t="s">
+        <v>267</v>
+      </c>
+      <c r="R74" s="15" t="s">
         <v>268</v>
       </c>
-      <c r="S74" s="32">
+      <c r="S74" s="15">
         <v>-124.1514</v>
       </c>
-      <c r="T74" s="32" t="s">
-        <v>267</v>
-      </c>
-      <c r="U74" s="32" t="s">
+      <c r="T74" s="15" t="s">
+        <v>267</v>
+      </c>
+      <c r="U74" s="15" t="s">
         <v>268</v>
       </c>
-      <c r="V74" s="32" t="s">
+      <c r="V74" s="15" t="s">
         <v>457</v>
       </c>
-      <c r="W74" s="32">
+      <c r="W74" s="15">
         <v>2014.0</v>
       </c>
-      <c r="X74" s="32" t="s">
-        <v>269</v>
-      </c>
-      <c r="AG74" s="32" t="s">
+      <c r="X74" s="15" t="s">
+        <v>269</v>
+      </c>
+      <c r="AG74" s="15" t="s">
         <v>431</v>
       </c>
-      <c r="AH74" s="32" t="s">
+      <c r="AH74" s="15" t="s">
         <v>263</v>
       </c>
-      <c r="AI74" s="32" t="s">
-        <v>264</v>
-      </c>
-      <c r="AJ74" s="32" t="s">
+      <c r="AI74" s="15" t="s">
+        <v>264</v>
+      </c>
+      <c r="AJ74" s="15" t="s">
         <v>265</v>
       </c>
-      <c r="AN74" s="32" t="s">
+      <c r="AN74" s="15" t="s">
         <v>456</v>
       </c>
-      <c r="AO74" s="32">
+      <c r="AO74" s="15">
         <v>41.0518</v>
       </c>
-      <c r="AP74" s="32" t="s">
-        <v>267</v>
-      </c>
-      <c r="AQ74" s="32" t="s">
+      <c r="AP74" s="15" t="s">
+        <v>267</v>
+      </c>
+      <c r="AQ74" s="15" t="s">
         <v>268</v>
       </c>
-      <c r="AR74" s="32">
+      <c r="AR74" s="15">
         <v>-124.1514</v>
       </c>
-      <c r="AS74" s="32" t="s">
-        <v>267</v>
-      </c>
-      <c r="AT74" s="32" t="s">
+      <c r="AS74" s="15" t="s">
+        <v>267</v>
+      </c>
+      <c r="AT74" s="15" t="s">
         <v>268</v>
       </c>
-      <c r="AU74" s="32" t="s">
+      <c r="AU74" s="15" t="s">
         <v>457</v>
       </c>
-      <c r="AV74" s="32">
+      <c r="AV74" s="15">
         <v>2015.0</v>
       </c>
-      <c r="AW74" s="32" t="s">
-        <v>269</v>
+      <c r="AW74" s="15" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="16">
+        <v>45859.69089540509</v>
+      </c>
+      <c r="B75" s="17" t="s">
+        <v>403</v>
+      </c>
+      <c r="C75" s="17" t="s">
+        <v>404</v>
+      </c>
+      <c r="D75" s="17">
+        <v>74.0</v>
+      </c>
+      <c r="E75" s="17" t="s">
+        <v>261</v>
+      </c>
+      <c r="H75" s="17" t="s">
+        <v>417</v>
+      </c>
+      <c r="I75" s="17" t="s">
+        <v>263</v>
+      </c>
+      <c r="J75" s="17" t="s">
+        <v>264</v>
+      </c>
+      <c r="K75" s="17" t="s">
+        <v>265</v>
+      </c>
+      <c r="L75" s="17" t="s">
+        <v>458</v>
+      </c>
+      <c r="M75" s="17" t="s">
+        <v>263</v>
+      </c>
+      <c r="N75" s="17" t="s">
+        <v>264</v>
+      </c>
+      <c r="O75" s="17" t="s">
+        <v>459</v>
+      </c>
+      <c r="P75" s="17">
+        <v>44.65</v>
+      </c>
+      <c r="Q75" s="17" t="s">
+        <v>269</v>
+      </c>
+      <c r="R75" s="17" t="s">
+        <v>264</v>
+      </c>
+      <c r="S75" s="17">
+        <v>-124.0</v>
+      </c>
+      <c r="T75" s="17" t="s">
+        <v>267</v>
+      </c>
+      <c r="U75" s="17" t="s">
+        <v>268</v>
+      </c>
+      <c r="V75" s="17" t="s">
+        <v>460</v>
+      </c>
+      <c r="W75" s="17">
+        <v>2016.0</v>
+      </c>
+      <c r="X75" s="17" t="s">
+        <v>269</v>
+      </c>
+      <c r="Y75" s="17" t="s">
+        <v>461</v>
+      </c>
+      <c r="Z75" s="17" t="s">
+        <v>284</v>
+      </c>
+      <c r="AC75" s="17" t="s">
+        <v>462</v>
+      </c>
+      <c r="AD75" s="17">
+        <v>32.5</v>
+      </c>
+      <c r="AE75" s="17" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="31">
+        <v>45859.69428454861</v>
+      </c>
+      <c r="B76" s="32" t="s">
+        <v>403</v>
+      </c>
+      <c r="C76" s="32" t="s">
+        <v>404</v>
+      </c>
+      <c r="D76" s="32">
+        <v>75.0</v>
+      </c>
+      <c r="E76" s="32" t="s">
+        <v>261</v>
+      </c>
+      <c r="H76" s="32" t="s">
+        <v>463</v>
+      </c>
+      <c r="I76" s="32" t="s">
+        <v>263</v>
+      </c>
+      <c r="J76" s="32" t="s">
+        <v>264</v>
+      </c>
+      <c r="K76" s="32" t="s">
+        <v>265</v>
+      </c>
+      <c r="O76" s="32" t="s">
+        <v>464</v>
+      </c>
+      <c r="P76" s="32">
+        <v>42.0</v>
+      </c>
+      <c r="Q76" s="32" t="s">
+        <v>267</v>
+      </c>
+      <c r="R76" s="32" t="s">
+        <v>264</v>
+      </c>
+      <c r="S76" s="32">
+        <v>-124.3</v>
+      </c>
+      <c r="T76" s="32" t="s">
+        <v>267</v>
+      </c>
+      <c r="U76" s="32" t="s">
+        <v>268</v>
+      </c>
+      <c r="V76" s="32">
+        <v>2015.0</v>
+      </c>
+      <c r="W76" s="32">
+        <v>2015.0</v>
+      </c>
+      <c r="X76" s="32" t="s">
+        <v>269</v>
+      </c>
+      <c r="AC76" s="32" t="s">
+        <v>465</v>
+      </c>
+      <c r="AG76" s="32" t="s">
+        <v>466</v>
+      </c>
+      <c r="AH76" s="32" t="s">
+        <v>263</v>
+      </c>
+      <c r="AI76" s="32" t="s">
+        <v>264</v>
+      </c>
+      <c r="AJ76" s="32" t="s">
+        <v>265</v>
+      </c>
+      <c r="AN76" s="32" t="s">
+        <v>464</v>
+      </c>
+      <c r="AO76" s="32">
+        <v>42.0</v>
+      </c>
+      <c r="AP76" s="32" t="s">
+        <v>267</v>
+      </c>
+      <c r="AQ76" s="32" t="s">
+        <v>264</v>
+      </c>
+      <c r="AR76" s="32">
+        <v>-124.3</v>
+      </c>
+      <c r="AS76" s="32" t="s">
+        <v>267</v>
+      </c>
+      <c r="AT76" s="32" t="s">
+        <v>268</v>
+      </c>
+      <c r="AU76" s="32">
+        <v>2015.0</v>
+      </c>
+      <c r="AV76" s="32">
+        <v>2015.0</v>
+      </c>
+      <c r="AW76" s="32" t="s">
+        <v>269</v>
+      </c>
+      <c r="BB76" s="32" t="s">
+        <v>465</v>
+      </c>
+      <c r="BF76" s="32" t="s">
+        <v>467</v>
+      </c>
+      <c r="BG76" s="32" t="s">
+        <v>263</v>
+      </c>
+      <c r="BH76" s="32" t="s">
+        <v>264</v>
+      </c>
+      <c r="BI76" s="32" t="s">
+        <v>360</v>
+      </c>
+      <c r="BM76" s="32" t="s">
+        <v>464</v>
+      </c>
+      <c r="BN76" s="32">
+        <v>42.0</v>
+      </c>
+      <c r="BO76" s="32" t="s">
+        <v>267</v>
+      </c>
+      <c r="BP76" s="32" t="s">
+        <v>264</v>
+      </c>
+      <c r="BQ76" s="32">
+        <v>-124.3</v>
+      </c>
+      <c r="BR76" s="32" t="s">
+        <v>267</v>
+      </c>
+      <c r="BS76" s="32" t="s">
+        <v>268</v>
+      </c>
+      <c r="BT76" s="32">
+        <v>2015.0</v>
+      </c>
+      <c r="BU76" s="32">
+        <v>2015.0</v>
+      </c>
+      <c r="BV76" s="32" t="s">
+        <v>269</v>
+      </c>
+      <c r="CA76" s="32" t="s">
+        <v>465</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
dropped the south dispersing jellyfish
</commit_message>
<xml_diff>
--- a/data/CalCOFI Coding Form (Responses).xlsx
+++ b/data/CalCOFI Coding Form (Responses).xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1689" uniqueCount="468">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1678" uniqueCount="467">
   <si>
     <t>Timestamp</t>
   </si>
@@ -1436,16 +1436,13 @@
     <t>tropical species</t>
   </si>
   <si>
-    <t>Phacellophora camchatica</t>
+    <t>Velella velella</t>
   </si>
   <si>
     <t>Northern California Current, Oregon and Washington Coast</t>
   </si>
   <si>
     <t>offshore and/or southern species</t>
-  </si>
-  <si>
-    <t>Velella velella</t>
   </si>
   <si>
     <t>Thetys</t>
@@ -1458,7 +1455,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yyyy h:mm:ss"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="9">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -1492,6 +1489,14 @@
     </font>
     <font>
       <sz val="12.0"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <color rgb="FF434343"/>
+      <name val="Roboto"/>
+    </font>
+    <font>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
@@ -1670,7 +1675,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="38">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1769,6 +1774,21 @@
     </xf>
     <xf borderId="11" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="11" fillId="2" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="11" fillId="2" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="11" fillId="2" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="right" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="11" fillId="2" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="11" fillId="2" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="right" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -10569,139 +10589,111 @@
       <c r="E76" s="32" t="s">
         <v>261</v>
       </c>
-      <c r="H76" s="32" t="s">
+      <c r="H76" s="33" t="s">
         <v>463</v>
       </c>
-      <c r="I76" s="32" t="s">
+      <c r="I76" s="33" t="s">
         <v>263</v>
       </c>
-      <c r="J76" s="32" t="s">
-        <v>264</v>
-      </c>
-      <c r="K76" s="32" t="s">
+      <c r="J76" s="33" t="s">
+        <v>264</v>
+      </c>
+      <c r="K76" s="33" t="s">
         <v>265</v>
       </c>
-      <c r="O76" s="32" t="s">
+      <c r="L76" s="34"/>
+      <c r="M76" s="34"/>
+      <c r="N76" s="34"/>
+      <c r="O76" s="33" t="s">
         <v>464</v>
       </c>
-      <c r="P76" s="32">
+      <c r="P76" s="35">
         <v>42.0</v>
       </c>
-      <c r="Q76" s="32" t="s">
-        <v>267</v>
-      </c>
-      <c r="R76" s="32" t="s">
-        <v>264</v>
-      </c>
-      <c r="S76" s="32">
+      <c r="Q76" s="33" t="s">
+        <v>267</v>
+      </c>
+      <c r="R76" s="33" t="s">
+        <v>264</v>
+      </c>
+      <c r="S76" s="35">
         <v>-124.3</v>
       </c>
-      <c r="T76" s="32" t="s">
-        <v>267</v>
-      </c>
-      <c r="U76" s="32" t="s">
+      <c r="T76" s="33" t="s">
+        <v>267</v>
+      </c>
+      <c r="U76" s="33" t="s">
         <v>268</v>
       </c>
-      <c r="V76" s="32">
+      <c r="V76" s="35">
         <v>2015.0</v>
       </c>
-      <c r="W76" s="32">
+      <c r="W76" s="35">
         <v>2015.0</v>
       </c>
-      <c r="X76" s="32" t="s">
-        <v>269</v>
-      </c>
-      <c r="AC76" s="32" t="s">
+      <c r="X76" s="33" t="s">
+        <v>269</v>
+      </c>
+      <c r="Y76" s="34"/>
+      <c r="Z76" s="34"/>
+      <c r="AA76" s="34"/>
+      <c r="AB76" s="34"/>
+      <c r="AC76" s="33" t="s">
         <v>465</v>
       </c>
-      <c r="AG76" s="32" t="s">
+      <c r="AD76" s="34"/>
+      <c r="AE76" s="34"/>
+      <c r="AF76" s="34"/>
+      <c r="AG76" s="36" t="s">
         <v>466</v>
       </c>
-      <c r="AH76" s="32" t="s">
+      <c r="AH76" s="36" t="s">
         <v>263</v>
       </c>
-      <c r="AI76" s="32" t="s">
-        <v>264</v>
-      </c>
-      <c r="AJ76" s="32" t="s">
-        <v>265</v>
-      </c>
-      <c r="AN76" s="32" t="s">
+      <c r="AI76" s="36" t="s">
+        <v>264</v>
+      </c>
+      <c r="AJ76" s="36" t="s">
+        <v>360</v>
+      </c>
+      <c r="AK76" s="34"/>
+      <c r="AL76" s="34"/>
+      <c r="AM76" s="34"/>
+      <c r="AN76" s="36" t="s">
         <v>464</v>
       </c>
-      <c r="AO76" s="32">
+      <c r="AO76" s="37">
         <v>42.0</v>
       </c>
-      <c r="AP76" s="32" t="s">
-        <v>267</v>
-      </c>
-      <c r="AQ76" s="32" t="s">
-        <v>264</v>
-      </c>
-      <c r="AR76" s="32">
+      <c r="AP76" s="36" t="s">
+        <v>267</v>
+      </c>
+      <c r="AQ76" s="36" t="s">
+        <v>264</v>
+      </c>
+      <c r="AR76" s="37">
         <v>-124.3</v>
       </c>
-      <c r="AS76" s="32" t="s">
-        <v>267</v>
-      </c>
-      <c r="AT76" s="32" t="s">
+      <c r="AS76" s="36" t="s">
+        <v>267</v>
+      </c>
+      <c r="AT76" s="36" t="s">
         <v>268</v>
       </c>
-      <c r="AU76" s="32">
+      <c r="AU76" s="37">
         <v>2015.0</v>
       </c>
-      <c r="AV76" s="32">
+      <c r="AV76" s="37">
         <v>2015.0</v>
       </c>
-      <c r="AW76" s="32" t="s">
-        <v>269</v>
-      </c>
-      <c r="BB76" s="32" t="s">
-        <v>465</v>
-      </c>
-      <c r="BF76" s="32" t="s">
-        <v>467</v>
-      </c>
-      <c r="BG76" s="32" t="s">
-        <v>263</v>
-      </c>
-      <c r="BH76" s="32" t="s">
-        <v>264</v>
-      </c>
-      <c r="BI76" s="32" t="s">
-        <v>360</v>
-      </c>
-      <c r="BM76" s="32" t="s">
-        <v>464</v>
-      </c>
-      <c r="BN76" s="32">
-        <v>42.0</v>
-      </c>
-      <c r="BO76" s="32" t="s">
-        <v>267</v>
-      </c>
-      <c r="BP76" s="32" t="s">
-        <v>264</v>
-      </c>
-      <c r="BQ76" s="32">
-        <v>-124.3</v>
-      </c>
-      <c r="BR76" s="32" t="s">
-        <v>267</v>
-      </c>
-      <c r="BS76" s="32" t="s">
-        <v>268</v>
-      </c>
-      <c r="BT76" s="32">
-        <v>2015.0</v>
-      </c>
-      <c r="BU76" s="32">
-        <v>2015.0</v>
-      </c>
-      <c r="BV76" s="32" t="s">
-        <v>269</v>
-      </c>
-      <c r="CA76" s="32" t="s">
+      <c r="AW76" s="36" t="s">
+        <v>269</v>
+      </c>
+      <c r="AX76" s="34"/>
+      <c r="AY76" s="34"/>
+      <c r="AZ76" s="34"/>
+      <c r="BA76" s="34"/>
+      <c r="BB76" s="36" t="s">
         <v>465</v>
       </c>
     </row>

</xml_diff>